<commit_message>
Add estate test evidence
</commit_message>
<xml_diff>
--- a/documentation/04_テスト/02_結合テスト_IT/01_テスト仕様書/管理者＿住宅＿テスト仕様書.xlsx
+++ b/documentation/04_テスト/02_結合テスト_IT/01_テスト仕様書/管理者＿住宅＿テスト仕様書.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFBDFF0D-FB1F-4CEE-A77D-37BE20DC8053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83219DE5-2C4B-4467-A6AE-FBDFFF4A4ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="961" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
   <si>
     <t>作成者</t>
     <rPh sb="0" eb="3">
@@ -305,6 +305,15 @@
   <si>
     <t>管理画面の住宅一覧に該当住宅が表示されること</t>
   </si>
+  <si>
+    <t>住宅を削除する</t>
+  </si>
+  <si>
+    <t>住宅を編集する</t>
+  </si>
+  <si>
+    <t>レイアウト</t>
+  </si>
 </sst>
 </file>
 
@@ -313,7 +322,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -415,6 +424,17 @@
       <name val="ＭＳ Ｐゴシック"/>
       <charset val="128"/>
     </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -694,7 +714,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -734,21 +754,138 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -761,123 +898,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -889,6 +909,12 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -909,156 +935,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>127000</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>52</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>190964</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1960563" y="1083468"/>
-          <a:ext cx="9909968" cy="4977277"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>118249</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>114281</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>52</xdr:col>
-      <xdr:colOff>276999</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>12467</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1951812" y="6186469"/>
-          <a:ext cx="9909968" cy="4958342"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>53</xdr:col>
-      <xdr:colOff>573049</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>68226</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>71</xdr:col>
-      <xdr:colOff>215068</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>195275</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12741237" y="1080257"/>
-          <a:ext cx="10143331" cy="4984799"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>73</xdr:col>
@@ -1086,7 +962,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1136,7 +1012,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1170,7 +1046,7 @@
       <xdr:col>109</xdr:col>
       <xdr:colOff>315818</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>106329</xdr:rowOff>
+      <xdr:rowOff>30129</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1186,7 +1062,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1219,8 +1095,8 @@
     <xdr:to>
       <xdr:col>126</xdr:col>
       <xdr:colOff>408535</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>133351</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1236,7 +1112,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1285,7 +1161,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1300,6 +1176,256 @@
         <a:xfrm>
           <a:off x="45405655" y="995342"/>
           <a:ext cx="10058400" cy="3409950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>48</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>42165</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF300132-8F86-464F-1644-55FB76C68E80}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="333375" y="1362075"/>
+          <a:ext cx="9639300" cy="4966590"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>26174</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>83325</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>48</xdr:col>
+      <xdr:colOff>478399</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6FFEBC8-3DCC-973E-69BB-FB4D197F8328}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="197624" y="7208025"/>
+          <a:ext cx="9767675" cy="4631550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>387866</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>4725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>67</xdr:col>
+      <xdr:colOff>519075</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F6A69EC-BEAF-912F-4FE8-CF4D2D2274B4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11646416" y="1262025"/>
+          <a:ext cx="9580009" cy="4872075"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>397035</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>59475</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>67</xdr:col>
+      <xdr:colOff>259500</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E22015BF-99D4-B8B0-5527-3FA28949C25F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11655585" y="7184175"/>
+          <a:ext cx="9311265" cy="4760175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>171375</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>114225</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>45</xdr:col>
+      <xdr:colOff>399975</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>119258</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C2C76FE-3678-759E-7C69-33F2E00A003E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="342825" y="12972975"/>
+          <a:ext cx="7772400" cy="4196033"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1817,924 +1943,924 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:71" ht="16.2" customHeight="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="35"/>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="39" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="S1" s="39"/>
-      <c r="T1" s="39"/>
-      <c r="U1" s="39"/>
-      <c r="V1" s="39"/>
-      <c r="W1" s="39"/>
-      <c r="X1" s="41" t="s">
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29"/>
+      <c r="X1" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="Y1" s="42"/>
-      <c r="Z1" s="42"/>
-      <c r="AA1" s="42"/>
-      <c r="AB1" s="42"/>
-      <c r="AC1" s="42"/>
-      <c r="AD1" s="42"/>
-      <c r="AE1" s="42"/>
-      <c r="AF1" s="42"/>
-      <c r="AG1" s="42"/>
-      <c r="AH1" s="42"/>
-      <c r="AI1" s="42"/>
-      <c r="AJ1" s="42"/>
-      <c r="AK1" s="42"/>
-      <c r="AL1" s="42"/>
-      <c r="AM1" s="42"/>
-      <c r="AN1" s="42"/>
-      <c r="AO1" s="42"/>
-      <c r="AP1" s="42"/>
-      <c r="AQ1" s="42"/>
-      <c r="AR1" s="42"/>
-      <c r="AS1" s="42"/>
-      <c r="AT1" s="42"/>
-      <c r="AU1" s="42"/>
-      <c r="AV1" s="42"/>
-      <c r="AW1" s="42"/>
-      <c r="AX1" s="42"/>
-      <c r="AY1" s="42"/>
-      <c r="AZ1" s="43"/>
-      <c r="BA1" s="47" t="s">
+      <c r="Y1" s="32"/>
+      <c r="Z1" s="32"/>
+      <c r="AA1" s="32"/>
+      <c r="AB1" s="32"/>
+      <c r="AC1" s="32"/>
+      <c r="AD1" s="32"/>
+      <c r="AE1" s="32"/>
+      <c r="AF1" s="32"/>
+      <c r="AG1" s="32"/>
+      <c r="AH1" s="32"/>
+      <c r="AI1" s="32"/>
+      <c r="AJ1" s="32"/>
+      <c r="AK1" s="32"/>
+      <c r="AL1" s="32"/>
+      <c r="AM1" s="32"/>
+      <c r="AN1" s="32"/>
+      <c r="AO1" s="32"/>
+      <c r="AP1" s="32"/>
+      <c r="AQ1" s="32"/>
+      <c r="AR1" s="32"/>
+      <c r="AS1" s="32"/>
+      <c r="AT1" s="32"/>
+      <c r="AU1" s="32"/>
+      <c r="AV1" s="32"/>
+      <c r="AW1" s="32"/>
+      <c r="AX1" s="32"/>
+      <c r="AY1" s="32"/>
+      <c r="AZ1" s="33"/>
+      <c r="BA1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="BB1" s="48"/>
-      <c r="BC1" s="49"/>
-      <c r="BD1" s="53">
+      <c r="BB1" s="38"/>
+      <c r="BC1" s="39"/>
+      <c r="BD1" s="43">
         <v>44892</v>
       </c>
-      <c r="BE1" s="54"/>
-      <c r="BF1" s="54"/>
-      <c r="BG1" s="54"/>
-      <c r="BH1" s="54"/>
-      <c r="BI1" s="55"/>
-      <c r="BJ1" s="59" t="s">
+      <c r="BE1" s="44"/>
+      <c r="BF1" s="44"/>
+      <c r="BG1" s="44"/>
+      <c r="BH1" s="44"/>
+      <c r="BI1" s="45"/>
+      <c r="BJ1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="BK1" s="48"/>
-      <c r="BL1" s="49"/>
-      <c r="BM1" s="23" t="s">
+      <c r="BK1" s="38"/>
+      <c r="BL1" s="39"/>
+      <c r="BM1" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="BN1" s="24"/>
-      <c r="BO1" s="24"/>
-      <c r="BP1" s="25"/>
+      <c r="BN1" s="14"/>
+      <c r="BO1" s="14"/>
+      <c r="BP1" s="15"/>
     </row>
     <row r="2" spans="1:71" ht="16.2" customHeight="1" thickBot="1">
-      <c r="A2" s="36"/>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
-      <c r="O2" s="38"/>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="38"/>
-      <c r="R2" s="40"/>
-      <c r="S2" s="40"/>
-      <c r="T2" s="40"/>
-      <c r="U2" s="40"/>
-      <c r="V2" s="40"/>
-      <c r="W2" s="40"/>
-      <c r="X2" s="44"/>
-      <c r="Y2" s="45"/>
-      <c r="Z2" s="45"/>
-      <c r="AA2" s="45"/>
-      <c r="AB2" s="45"/>
-      <c r="AC2" s="45"/>
-      <c r="AD2" s="45"/>
-      <c r="AE2" s="45"/>
-      <c r="AF2" s="45"/>
-      <c r="AG2" s="45"/>
-      <c r="AH2" s="45"/>
-      <c r="AI2" s="45"/>
-      <c r="AJ2" s="45"/>
-      <c r="AK2" s="45"/>
-      <c r="AL2" s="45"/>
-      <c r="AM2" s="45"/>
-      <c r="AN2" s="45"/>
-      <c r="AO2" s="45"/>
-      <c r="AP2" s="45"/>
-      <c r="AQ2" s="45"/>
-      <c r="AR2" s="45"/>
-      <c r="AS2" s="45"/>
-      <c r="AT2" s="45"/>
-      <c r="AU2" s="45"/>
-      <c r="AV2" s="45"/>
-      <c r="AW2" s="45"/>
-      <c r="AX2" s="45"/>
-      <c r="AY2" s="45"/>
-      <c r="AZ2" s="46"/>
-      <c r="BA2" s="50"/>
-      <c r="BB2" s="51"/>
-      <c r="BC2" s="52"/>
-      <c r="BD2" s="56"/>
-      <c r="BE2" s="57"/>
-      <c r="BF2" s="57"/>
-      <c r="BG2" s="57"/>
-      <c r="BH2" s="57"/>
-      <c r="BI2" s="58"/>
-      <c r="BJ2" s="60"/>
-      <c r="BK2" s="51"/>
-      <c r="BL2" s="52"/>
-      <c r="BM2" s="26"/>
-      <c r="BN2" s="27"/>
-      <c r="BO2" s="27"/>
-      <c r="BP2" s="28"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="28"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="30"/>
+      <c r="V2" s="30"/>
+      <c r="W2" s="30"/>
+      <c r="X2" s="34"/>
+      <c r="Y2" s="35"/>
+      <c r="Z2" s="35"/>
+      <c r="AA2" s="35"/>
+      <c r="AB2" s="35"/>
+      <c r="AC2" s="35"/>
+      <c r="AD2" s="35"/>
+      <c r="AE2" s="35"/>
+      <c r="AF2" s="35"/>
+      <c r="AG2" s="35"/>
+      <c r="AH2" s="35"/>
+      <c r="AI2" s="35"/>
+      <c r="AJ2" s="35"/>
+      <c r="AK2" s="35"/>
+      <c r="AL2" s="35"/>
+      <c r="AM2" s="35"/>
+      <c r="AN2" s="35"/>
+      <c r="AO2" s="35"/>
+      <c r="AP2" s="35"/>
+      <c r="AQ2" s="35"/>
+      <c r="AR2" s="35"/>
+      <c r="AS2" s="35"/>
+      <c r="AT2" s="35"/>
+      <c r="AU2" s="35"/>
+      <c r="AV2" s="35"/>
+      <c r="AW2" s="35"/>
+      <c r="AX2" s="35"/>
+      <c r="AY2" s="35"/>
+      <c r="AZ2" s="36"/>
+      <c r="BA2" s="40"/>
+      <c r="BB2" s="41"/>
+      <c r="BC2" s="42"/>
+      <c r="BD2" s="46"/>
+      <c r="BE2" s="47"/>
+      <c r="BF2" s="47"/>
+      <c r="BG2" s="47"/>
+      <c r="BH2" s="47"/>
+      <c r="BI2" s="48"/>
+      <c r="BJ2" s="50"/>
+      <c r="BK2" s="41"/>
+      <c r="BL2" s="42"/>
+      <c r="BM2" s="16"/>
+      <c r="BN2" s="17"/>
+      <c r="BO2" s="17"/>
+      <c r="BP2" s="18"/>
     </row>
     <row r="3" spans="1:71" ht="8.1" customHeight="1"/>
     <row r="4" spans="1:71" s="2" customFormat="1" ht="16.2" customHeight="1">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29" t="s">
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="30" t="s">
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="31"/>
-      <c r="L4" s="31"/>
-      <c r="M4" s="31"/>
-      <c r="N4" s="31"/>
-      <c r="O4" s="31"/>
-      <c r="P4" s="31"/>
-      <c r="Q4" s="31"/>
-      <c r="R4" s="31"/>
-      <c r="S4" s="32"/>
-      <c r="T4" s="29" t="s">
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="21"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="21"/>
+      <c r="R4" s="21"/>
+      <c r="S4" s="22"/>
+      <c r="T4" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="U4" s="29"/>
-      <c r="V4" s="29"/>
-      <c r="W4" s="29"/>
-      <c r="X4" s="29"/>
-      <c r="Y4" s="29"/>
-      <c r="Z4" s="29"/>
-      <c r="AA4" s="29"/>
-      <c r="AB4" s="29"/>
-      <c r="AC4" s="29"/>
-      <c r="AD4" s="29"/>
-      <c r="AE4" s="29"/>
-      <c r="AF4" s="29"/>
-      <c r="AG4" s="29"/>
-      <c r="AH4" s="29"/>
-      <c r="AI4" s="29" t="s">
+      <c r="U4" s="19"/>
+      <c r="V4" s="19"/>
+      <c r="W4" s="19"/>
+      <c r="X4" s="19"/>
+      <c r="Y4" s="19"/>
+      <c r="Z4" s="19"/>
+      <c r="AA4" s="19"/>
+      <c r="AB4" s="19"/>
+      <c r="AC4" s="19"/>
+      <c r="AD4" s="19"/>
+      <c r="AE4" s="19"/>
+      <c r="AF4" s="19"/>
+      <c r="AG4" s="19"/>
+      <c r="AH4" s="19"/>
+      <c r="AI4" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="AJ4" s="29"/>
-      <c r="AK4" s="29"/>
-      <c r="AL4" s="29"/>
-      <c r="AM4" s="29"/>
-      <c r="AN4" s="29"/>
-      <c r="AO4" s="29"/>
-      <c r="AP4" s="29"/>
-      <c r="AQ4" s="29"/>
-      <c r="AR4" s="29"/>
-      <c r="AS4" s="29"/>
-      <c r="AT4" s="29"/>
-      <c r="AU4" s="29"/>
-      <c r="AV4" s="29"/>
-      <c r="AW4" s="29"/>
-      <c r="AX4" s="29"/>
-      <c r="AY4" s="29"/>
-      <c r="AZ4" s="29"/>
-      <c r="BA4" s="29"/>
-      <c r="BB4" s="29"/>
-      <c r="BC4" s="29"/>
-      <c r="BD4" s="29" t="s">
+      <c r="AJ4" s="19"/>
+      <c r="AK4" s="19"/>
+      <c r="AL4" s="19"/>
+      <c r="AM4" s="19"/>
+      <c r="AN4" s="19"/>
+      <c r="AO4" s="19"/>
+      <c r="AP4" s="19"/>
+      <c r="AQ4" s="19"/>
+      <c r="AR4" s="19"/>
+      <c r="AS4" s="19"/>
+      <c r="AT4" s="19"/>
+      <c r="AU4" s="19"/>
+      <c r="AV4" s="19"/>
+      <c r="AW4" s="19"/>
+      <c r="AX4" s="19"/>
+      <c r="AY4" s="19"/>
+      <c r="AZ4" s="19"/>
+      <c r="BA4" s="19"/>
+      <c r="BB4" s="19"/>
+      <c r="BC4" s="19"/>
+      <c r="BD4" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="BE4" s="29"/>
-      <c r="BF4" s="29"/>
-      <c r="BG4" s="29" t="s">
+      <c r="BE4" s="19"/>
+      <c r="BF4" s="19"/>
+      <c r="BG4" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="BH4" s="29"/>
-      <c r="BI4" s="29"/>
-      <c r="BJ4" s="29" t="s">
+      <c r="BH4" s="19"/>
+      <c r="BI4" s="19"/>
+      <c r="BJ4" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="BK4" s="29"/>
-      <c r="BL4" s="29" t="s">
+      <c r="BK4" s="19"/>
+      <c r="BL4" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="BM4" s="29"/>
-      <c r="BN4" s="29"/>
-      <c r="BO4" s="29" t="s">
+      <c r="BM4" s="19"/>
+      <c r="BN4" s="19"/>
+      <c r="BO4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="BP4" s="29"/>
+      <c r="BP4" s="19"/>
     </row>
     <row r="5" spans="1:71" ht="72" customHeight="1">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="15" t="s">
+      <c r="B5" s="51"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15" t="s">
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15" t="s">
+      <c r="K5" s="52"/>
+      <c r="L5" s="52"/>
+      <c r="M5" s="52"/>
+      <c r="N5" s="52"/>
+      <c r="O5" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="15"/>
-      <c r="S5" s="15"/>
-      <c r="T5" s="15" t="s">
+      <c r="P5" s="52"/>
+      <c r="Q5" s="52"/>
+      <c r="R5" s="52"/>
+      <c r="S5" s="52"/>
+      <c r="T5" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="U5" s="15"/>
-      <c r="V5" s="15"/>
-      <c r="W5" s="15"/>
-      <c r="X5" s="15"/>
-      <c r="Y5" s="15"/>
-      <c r="Z5" s="15"/>
-      <c r="AA5" s="15"/>
-      <c r="AB5" s="15"/>
-      <c r="AC5" s="15"/>
-      <c r="AD5" s="15"/>
-      <c r="AE5" s="15"/>
-      <c r="AF5" s="15"/>
-      <c r="AG5" s="15"/>
-      <c r="AH5" s="15"/>
-      <c r="AI5" s="15" t="s">
+      <c r="U5" s="52"/>
+      <c r="V5" s="52"/>
+      <c r="W5" s="52"/>
+      <c r="X5" s="52"/>
+      <c r="Y5" s="52"/>
+      <c r="Z5" s="52"/>
+      <c r="AA5" s="52"/>
+      <c r="AB5" s="52"/>
+      <c r="AC5" s="52"/>
+      <c r="AD5" s="52"/>
+      <c r="AE5" s="52"/>
+      <c r="AF5" s="52"/>
+      <c r="AG5" s="52"/>
+      <c r="AH5" s="52"/>
+      <c r="AI5" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="AJ5" s="15"/>
-      <c r="AK5" s="15"/>
-      <c r="AL5" s="15"/>
-      <c r="AM5" s="15"/>
-      <c r="AN5" s="15"/>
-      <c r="AO5" s="15"/>
-      <c r="AP5" s="15"/>
-      <c r="AQ5" s="15"/>
-      <c r="AR5" s="15"/>
-      <c r="AS5" s="15"/>
-      <c r="AT5" s="15"/>
-      <c r="AU5" s="15"/>
-      <c r="AV5" s="15"/>
-      <c r="AW5" s="15"/>
-      <c r="AX5" s="15"/>
-      <c r="AY5" s="15"/>
-      <c r="AZ5" s="15"/>
-      <c r="BA5" s="15"/>
-      <c r="BB5" s="15"/>
-      <c r="BC5" s="15"/>
-      <c r="BD5" s="22" t="s">
+      <c r="AJ5" s="52"/>
+      <c r="AK5" s="52"/>
+      <c r="AL5" s="52"/>
+      <c r="AM5" s="52"/>
+      <c r="AN5" s="52"/>
+      <c r="AO5" s="52"/>
+      <c r="AP5" s="52"/>
+      <c r="AQ5" s="52"/>
+      <c r="AR5" s="52"/>
+      <c r="AS5" s="52"/>
+      <c r="AT5" s="52"/>
+      <c r="AU5" s="52"/>
+      <c r="AV5" s="52"/>
+      <c r="AW5" s="52"/>
+      <c r="AX5" s="52"/>
+      <c r="AY5" s="52"/>
+      <c r="AZ5" s="52"/>
+      <c r="BA5" s="52"/>
+      <c r="BB5" s="52"/>
+      <c r="BC5" s="52"/>
+      <c r="BD5" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="BE5" s="16"/>
-      <c r="BF5" s="16"/>
-      <c r="BG5" s="13">
+      <c r="BE5" s="54"/>
+      <c r="BF5" s="54"/>
+      <c r="BG5" s="55">
         <v>44892</v>
       </c>
-      <c r="BH5" s="13"/>
-      <c r="BI5" s="13"/>
-      <c r="BJ5" s="14" t="s">
+      <c r="BH5" s="55"/>
+      <c r="BI5" s="55"/>
+      <c r="BJ5" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="BK5" s="14"/>
-      <c r="BL5" s="14"/>
-      <c r="BM5" s="14"/>
-      <c r="BN5" s="14"/>
-      <c r="BO5" s="13"/>
-      <c r="BP5" s="13"/>
+      <c r="BK5" s="56"/>
+      <c r="BL5" s="56"/>
+      <c r="BM5" s="56"/>
+      <c r="BN5" s="56"/>
+      <c r="BO5" s="55"/>
+      <c r="BP5" s="55"/>
       <c r="BS5" s="3"/>
     </row>
     <row r="6" spans="1:71" ht="72" customHeight="1">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="15" t="s">
+      <c r="B6" s="51"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15" t="s">
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15" t="s">
+      <c r="K6" s="52"/>
+      <c r="L6" s="52"/>
+      <c r="M6" s="52"/>
+      <c r="N6" s="52"/>
+      <c r="O6" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="15"/>
-      <c r="S6" s="15"/>
-      <c r="T6" s="15" t="s">
+      <c r="P6" s="52"/>
+      <c r="Q6" s="52"/>
+      <c r="R6" s="52"/>
+      <c r="S6" s="52"/>
+      <c r="T6" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="U6" s="15"/>
-      <c r="V6" s="15"/>
-      <c r="W6" s="15"/>
-      <c r="X6" s="15"/>
-      <c r="Y6" s="15"/>
-      <c r="Z6" s="15"/>
-      <c r="AA6" s="15"/>
-      <c r="AB6" s="15"/>
-      <c r="AC6" s="15"/>
-      <c r="AD6" s="15"/>
-      <c r="AE6" s="15"/>
-      <c r="AF6" s="15"/>
-      <c r="AG6" s="15"/>
-      <c r="AH6" s="15"/>
-      <c r="AI6" s="15" t="s">
+      <c r="U6" s="52"/>
+      <c r="V6" s="52"/>
+      <c r="W6" s="52"/>
+      <c r="X6" s="52"/>
+      <c r="Y6" s="52"/>
+      <c r="Z6" s="52"/>
+      <c r="AA6" s="52"/>
+      <c r="AB6" s="52"/>
+      <c r="AC6" s="52"/>
+      <c r="AD6" s="52"/>
+      <c r="AE6" s="52"/>
+      <c r="AF6" s="52"/>
+      <c r="AG6" s="52"/>
+      <c r="AH6" s="52"/>
+      <c r="AI6" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="AJ6" s="15"/>
-      <c r="AK6" s="15"/>
-      <c r="AL6" s="15"/>
-      <c r="AM6" s="15"/>
-      <c r="AN6" s="15"/>
-      <c r="AO6" s="15"/>
-      <c r="AP6" s="15"/>
-      <c r="AQ6" s="15"/>
-      <c r="AR6" s="15"/>
-      <c r="AS6" s="15"/>
-      <c r="AT6" s="15"/>
-      <c r="AU6" s="15"/>
-      <c r="AV6" s="15"/>
-      <c r="AW6" s="15"/>
-      <c r="AX6" s="15"/>
-      <c r="AY6" s="15"/>
-      <c r="AZ6" s="15"/>
-      <c r="BA6" s="15"/>
-      <c r="BB6" s="15"/>
-      <c r="BC6" s="15"/>
-      <c r="BD6" s="16"/>
-      <c r="BE6" s="16"/>
-      <c r="BF6" s="16"/>
-      <c r="BG6" s="13"/>
-      <c r="BH6" s="13"/>
-      <c r="BI6" s="13"/>
-      <c r="BJ6" s="14"/>
-      <c r="BK6" s="14"/>
-      <c r="BL6" s="14"/>
-      <c r="BM6" s="14"/>
-      <c r="BN6" s="14"/>
-      <c r="BO6" s="13"/>
-      <c r="BP6" s="13"/>
+      <c r="AJ6" s="52"/>
+      <c r="AK6" s="52"/>
+      <c r="AL6" s="52"/>
+      <c r="AM6" s="52"/>
+      <c r="AN6" s="52"/>
+      <c r="AO6" s="52"/>
+      <c r="AP6" s="52"/>
+      <c r="AQ6" s="52"/>
+      <c r="AR6" s="52"/>
+      <c r="AS6" s="52"/>
+      <c r="AT6" s="52"/>
+      <c r="AU6" s="52"/>
+      <c r="AV6" s="52"/>
+      <c r="AW6" s="52"/>
+      <c r="AX6" s="52"/>
+      <c r="AY6" s="52"/>
+      <c r="AZ6" s="52"/>
+      <c r="BA6" s="52"/>
+      <c r="BB6" s="52"/>
+      <c r="BC6" s="52"/>
+      <c r="BD6" s="54"/>
+      <c r="BE6" s="54"/>
+      <c r="BF6" s="54"/>
+      <c r="BG6" s="55"/>
+      <c r="BH6" s="55"/>
+      <c r="BI6" s="55"/>
+      <c r="BJ6" s="56"/>
+      <c r="BK6" s="56"/>
+      <c r="BL6" s="56"/>
+      <c r="BM6" s="56"/>
+      <c r="BN6" s="56"/>
+      <c r="BO6" s="55"/>
+      <c r="BP6" s="55"/>
       <c r="BS6" s="3"/>
     </row>
     <row r="7" spans="1:71" ht="72" customHeight="1">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="15" t="s">
+      <c r="B7" s="51"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15" t="s">
+      <c r="F7" s="52"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="52"/>
+      <c r="J7" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="15" t="s">
+      <c r="K7" s="52"/>
+      <c r="L7" s="52"/>
+      <c r="M7" s="52"/>
+      <c r="N7" s="52"/>
+      <c r="O7" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="P7" s="15"/>
-      <c r="Q7" s="15"/>
-      <c r="R7" s="15"/>
-      <c r="S7" s="15"/>
-      <c r="T7" s="15" t="s">
+      <c r="P7" s="52"/>
+      <c r="Q7" s="52"/>
+      <c r="R7" s="52"/>
+      <c r="S7" s="52"/>
+      <c r="T7" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="U7" s="15"/>
-      <c r="V7" s="15"/>
-      <c r="W7" s="15"/>
-      <c r="X7" s="15"/>
-      <c r="Y7" s="15"/>
-      <c r="Z7" s="15"/>
-      <c r="AA7" s="15"/>
-      <c r="AB7" s="15"/>
-      <c r="AC7" s="15"/>
-      <c r="AD7" s="15"/>
-      <c r="AE7" s="15"/>
-      <c r="AF7" s="15"/>
-      <c r="AG7" s="15"/>
-      <c r="AH7" s="15"/>
-      <c r="AI7" s="15" t="s">
+      <c r="U7" s="52"/>
+      <c r="V7" s="52"/>
+      <c r="W7" s="52"/>
+      <c r="X7" s="52"/>
+      <c r="Y7" s="52"/>
+      <c r="Z7" s="52"/>
+      <c r="AA7" s="52"/>
+      <c r="AB7" s="52"/>
+      <c r="AC7" s="52"/>
+      <c r="AD7" s="52"/>
+      <c r="AE7" s="52"/>
+      <c r="AF7" s="52"/>
+      <c r="AG7" s="52"/>
+      <c r="AH7" s="52"/>
+      <c r="AI7" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="AJ7" s="15"/>
-      <c r="AK7" s="15"/>
-      <c r="AL7" s="15"/>
-      <c r="AM7" s="15"/>
-      <c r="AN7" s="15"/>
-      <c r="AO7" s="15"/>
-      <c r="AP7" s="15"/>
-      <c r="AQ7" s="15"/>
-      <c r="AR7" s="15"/>
-      <c r="AS7" s="15"/>
-      <c r="AT7" s="15"/>
-      <c r="AU7" s="15"/>
-      <c r="AV7" s="15"/>
-      <c r="AW7" s="15"/>
-      <c r="AX7" s="15"/>
-      <c r="AY7" s="15"/>
-      <c r="AZ7" s="15"/>
-      <c r="BA7" s="15"/>
-      <c r="BB7" s="15"/>
-      <c r="BC7" s="15"/>
-      <c r="BD7" s="16"/>
-      <c r="BE7" s="16"/>
-      <c r="BF7" s="16"/>
-      <c r="BG7" s="13"/>
-      <c r="BH7" s="13"/>
-      <c r="BI7" s="13"/>
-      <c r="BJ7" s="14"/>
-      <c r="BK7" s="14"/>
-      <c r="BL7" s="14"/>
-      <c r="BM7" s="14"/>
-      <c r="BN7" s="14"/>
-      <c r="BO7" s="13"/>
-      <c r="BP7" s="13"/>
+      <c r="AJ7" s="52"/>
+      <c r="AK7" s="52"/>
+      <c r="AL7" s="52"/>
+      <c r="AM7" s="52"/>
+      <c r="AN7" s="52"/>
+      <c r="AO7" s="52"/>
+      <c r="AP7" s="52"/>
+      <c r="AQ7" s="52"/>
+      <c r="AR7" s="52"/>
+      <c r="AS7" s="52"/>
+      <c r="AT7" s="52"/>
+      <c r="AU7" s="52"/>
+      <c r="AV7" s="52"/>
+      <c r="AW7" s="52"/>
+      <c r="AX7" s="52"/>
+      <c r="AY7" s="52"/>
+      <c r="AZ7" s="52"/>
+      <c r="BA7" s="52"/>
+      <c r="BB7" s="52"/>
+      <c r="BC7" s="52"/>
+      <c r="BD7" s="54"/>
+      <c r="BE7" s="54"/>
+      <c r="BF7" s="54"/>
+      <c r="BG7" s="55"/>
+      <c r="BH7" s="55"/>
+      <c r="BI7" s="55"/>
+      <c r="BJ7" s="56"/>
+      <c r="BK7" s="56"/>
+      <c r="BL7" s="56"/>
+      <c r="BM7" s="56"/>
+      <c r="BN7" s="56"/>
+      <c r="BO7" s="55"/>
+      <c r="BP7" s="55"/>
       <c r="BS7" s="3"/>
     </row>
     <row r="8" spans="1:71" ht="75" customHeight="1">
-      <c r="A8" s="17"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="15"/>
-      <c r="R8" s="15"/>
-      <c r="S8" s="15"/>
-      <c r="T8" s="15"/>
-      <c r="U8" s="15"/>
-      <c r="V8" s="15"/>
-      <c r="W8" s="15"/>
-      <c r="X8" s="15"/>
-      <c r="Y8" s="15"/>
-      <c r="Z8" s="15"/>
-      <c r="AA8" s="15"/>
-      <c r="AB8" s="15"/>
-      <c r="AC8" s="15"/>
-      <c r="AD8" s="15"/>
-      <c r="AE8" s="15"/>
-      <c r="AF8" s="15"/>
-      <c r="AG8" s="15"/>
-      <c r="AH8" s="15"/>
-      <c r="AI8" s="15"/>
-      <c r="AJ8" s="15"/>
-      <c r="AK8" s="15"/>
-      <c r="AL8" s="15"/>
-      <c r="AM8" s="15"/>
-      <c r="AN8" s="15"/>
-      <c r="AO8" s="15"/>
-      <c r="AP8" s="15"/>
-      <c r="AQ8" s="15"/>
-      <c r="AR8" s="15"/>
-      <c r="AS8" s="15"/>
-      <c r="AT8" s="15"/>
-      <c r="AU8" s="15"/>
-      <c r="AV8" s="15"/>
-      <c r="AW8" s="15"/>
-      <c r="AX8" s="15"/>
-      <c r="AY8" s="15"/>
-      <c r="AZ8" s="15"/>
-      <c r="BA8" s="15"/>
-      <c r="BB8" s="15"/>
-      <c r="BC8" s="15"/>
-      <c r="BD8" s="16"/>
-      <c r="BE8" s="16"/>
-      <c r="BF8" s="16"/>
-      <c r="BG8" s="13"/>
-      <c r="BH8" s="13"/>
-      <c r="BI8" s="13"/>
-      <c r="BJ8" s="14"/>
-      <c r="BK8" s="14"/>
-      <c r="BL8" s="14"/>
-      <c r="BM8" s="14"/>
-      <c r="BN8" s="14"/>
-      <c r="BO8" s="13"/>
-      <c r="BP8" s="13"/>
+      <c r="A8" s="51"/>
+      <c r="B8" s="51"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="52"/>
+      <c r="J8" s="52"/>
+      <c r="K8" s="52"/>
+      <c r="L8" s="52"/>
+      <c r="M8" s="52"/>
+      <c r="N8" s="52"/>
+      <c r="O8" s="52"/>
+      <c r="P8" s="52"/>
+      <c r="Q8" s="52"/>
+      <c r="R8" s="52"/>
+      <c r="S8" s="52"/>
+      <c r="T8" s="52"/>
+      <c r="U8" s="52"/>
+      <c r="V8" s="52"/>
+      <c r="W8" s="52"/>
+      <c r="X8" s="52"/>
+      <c r="Y8" s="52"/>
+      <c r="Z8" s="52"/>
+      <c r="AA8" s="52"/>
+      <c r="AB8" s="52"/>
+      <c r="AC8" s="52"/>
+      <c r="AD8" s="52"/>
+      <c r="AE8" s="52"/>
+      <c r="AF8" s="52"/>
+      <c r="AG8" s="52"/>
+      <c r="AH8" s="52"/>
+      <c r="AI8" s="52"/>
+      <c r="AJ8" s="52"/>
+      <c r="AK8" s="52"/>
+      <c r="AL8" s="52"/>
+      <c r="AM8" s="52"/>
+      <c r="AN8" s="52"/>
+      <c r="AO8" s="52"/>
+      <c r="AP8" s="52"/>
+      <c r="AQ8" s="52"/>
+      <c r="AR8" s="52"/>
+      <c r="AS8" s="52"/>
+      <c r="AT8" s="52"/>
+      <c r="AU8" s="52"/>
+      <c r="AV8" s="52"/>
+      <c r="AW8" s="52"/>
+      <c r="AX8" s="52"/>
+      <c r="AY8" s="52"/>
+      <c r="AZ8" s="52"/>
+      <c r="BA8" s="52"/>
+      <c r="BB8" s="52"/>
+      <c r="BC8" s="52"/>
+      <c r="BD8" s="54"/>
+      <c r="BE8" s="54"/>
+      <c r="BF8" s="54"/>
+      <c r="BG8" s="55"/>
+      <c r="BH8" s="55"/>
+      <c r="BI8" s="55"/>
+      <c r="BJ8" s="56"/>
+      <c r="BK8" s="56"/>
+      <c r="BL8" s="56"/>
+      <c r="BM8" s="56"/>
+      <c r="BN8" s="56"/>
+      <c r="BO8" s="55"/>
+      <c r="BP8" s="55"/>
     </row>
     <row r="9" spans="1:71" ht="16.2" customHeight="1">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="20"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="15"/>
-      <c r="Q9" s="15"/>
-      <c r="R9" s="15"/>
-      <c r="S9" s="15"/>
-      <c r="T9" s="15"/>
-      <c r="U9" s="15"/>
-      <c r="V9" s="15"/>
-      <c r="W9" s="15"/>
-      <c r="X9" s="15"/>
-      <c r="Y9" s="15"/>
-      <c r="Z9" s="15"/>
-      <c r="AA9" s="15"/>
-      <c r="AB9" s="15"/>
-      <c r="AC9" s="15"/>
-      <c r="AD9" s="15"/>
-      <c r="AE9" s="15"/>
-      <c r="AF9" s="15"/>
-      <c r="AG9" s="15"/>
-      <c r="AH9" s="15"/>
-      <c r="AI9" s="15"/>
-      <c r="AJ9" s="15"/>
-      <c r="AK9" s="15"/>
-      <c r="AL9" s="15"/>
-      <c r="AM9" s="15"/>
-      <c r="AN9" s="15"/>
-      <c r="AO9" s="15"/>
-      <c r="AP9" s="15"/>
-      <c r="AQ9" s="15"/>
-      <c r="AR9" s="15"/>
-      <c r="AS9" s="15"/>
-      <c r="AT9" s="15"/>
-      <c r="AU9" s="15"/>
-      <c r="AV9" s="15"/>
-      <c r="AW9" s="15"/>
-      <c r="AX9" s="15"/>
-      <c r="AY9" s="15"/>
-      <c r="AZ9" s="15"/>
-      <c r="BA9" s="15"/>
-      <c r="BB9" s="15"/>
-      <c r="BC9" s="15"/>
-      <c r="BD9" s="16"/>
-      <c r="BE9" s="16"/>
-      <c r="BF9" s="16"/>
-      <c r="BG9" s="13"/>
-      <c r="BH9" s="13"/>
-      <c r="BI9" s="13"/>
-      <c r="BJ9" s="14"/>
-      <c r="BK9" s="14"/>
-      <c r="BL9" s="14"/>
-      <c r="BM9" s="14"/>
-      <c r="BN9" s="14"/>
-      <c r="BO9" s="13"/>
-      <c r="BP9" s="13"/>
+      <c r="A9" s="51"/>
+      <c r="B9" s="51"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="60"/>
+      <c r="I9" s="60"/>
+      <c r="J9" s="57"/>
+      <c r="K9" s="58"/>
+      <c r="L9" s="58"/>
+      <c r="M9" s="58"/>
+      <c r="N9" s="59"/>
+      <c r="O9" s="52"/>
+      <c r="P9" s="52"/>
+      <c r="Q9" s="52"/>
+      <c r="R9" s="52"/>
+      <c r="S9" s="52"/>
+      <c r="T9" s="52"/>
+      <c r="U9" s="52"/>
+      <c r="V9" s="52"/>
+      <c r="W9" s="52"/>
+      <c r="X9" s="52"/>
+      <c r="Y9" s="52"/>
+      <c r="Z9" s="52"/>
+      <c r="AA9" s="52"/>
+      <c r="AB9" s="52"/>
+      <c r="AC9" s="52"/>
+      <c r="AD9" s="52"/>
+      <c r="AE9" s="52"/>
+      <c r="AF9" s="52"/>
+      <c r="AG9" s="52"/>
+      <c r="AH9" s="52"/>
+      <c r="AI9" s="52"/>
+      <c r="AJ9" s="52"/>
+      <c r="AK9" s="52"/>
+      <c r="AL9" s="52"/>
+      <c r="AM9" s="52"/>
+      <c r="AN9" s="52"/>
+      <c r="AO9" s="52"/>
+      <c r="AP9" s="52"/>
+      <c r="AQ9" s="52"/>
+      <c r="AR9" s="52"/>
+      <c r="AS9" s="52"/>
+      <c r="AT9" s="52"/>
+      <c r="AU9" s="52"/>
+      <c r="AV9" s="52"/>
+      <c r="AW9" s="52"/>
+      <c r="AX9" s="52"/>
+      <c r="AY9" s="52"/>
+      <c r="AZ9" s="52"/>
+      <c r="BA9" s="52"/>
+      <c r="BB9" s="52"/>
+      <c r="BC9" s="52"/>
+      <c r="BD9" s="54"/>
+      <c r="BE9" s="54"/>
+      <c r="BF9" s="54"/>
+      <c r="BG9" s="55"/>
+      <c r="BH9" s="55"/>
+      <c r="BI9" s="55"/>
+      <c r="BJ9" s="56"/>
+      <c r="BK9" s="56"/>
+      <c r="BL9" s="56"/>
+      <c r="BM9" s="56"/>
+      <c r="BN9" s="56"/>
+      <c r="BO9" s="55"/>
+      <c r="BP9" s="55"/>
     </row>
     <row r="10" spans="1:71" ht="16.2" customHeight="1">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="20"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="15"/>
-      <c r="R10" s="15"/>
-      <c r="S10" s="15"/>
-      <c r="T10" s="15"/>
-      <c r="U10" s="15"/>
-      <c r="V10" s="15"/>
-      <c r="W10" s="15"/>
-      <c r="X10" s="15"/>
-      <c r="Y10" s="15"/>
-      <c r="Z10" s="15"/>
-      <c r="AA10" s="15"/>
-      <c r="AB10" s="15"/>
-      <c r="AC10" s="15"/>
-      <c r="AD10" s="15"/>
-      <c r="AE10" s="15"/>
-      <c r="AF10" s="15"/>
-      <c r="AG10" s="15"/>
-      <c r="AH10" s="15"/>
-      <c r="AI10" s="15"/>
-      <c r="AJ10" s="15"/>
-      <c r="AK10" s="15"/>
-      <c r="AL10" s="15"/>
-      <c r="AM10" s="15"/>
-      <c r="AN10" s="15"/>
-      <c r="AO10" s="15"/>
-      <c r="AP10" s="15"/>
-      <c r="AQ10" s="15"/>
-      <c r="AR10" s="15"/>
-      <c r="AS10" s="15"/>
-      <c r="AT10" s="15"/>
-      <c r="AU10" s="15"/>
-      <c r="AV10" s="15"/>
-      <c r="AW10" s="15"/>
-      <c r="AX10" s="15"/>
-      <c r="AY10" s="15"/>
-      <c r="AZ10" s="15"/>
-      <c r="BA10" s="15"/>
-      <c r="BB10" s="15"/>
-      <c r="BC10" s="15"/>
-      <c r="BD10" s="16"/>
-      <c r="BE10" s="16"/>
-      <c r="BF10" s="16"/>
-      <c r="BG10" s="13"/>
-      <c r="BH10" s="13"/>
-      <c r="BI10" s="13"/>
-      <c r="BJ10" s="14"/>
-      <c r="BK10" s="14"/>
-      <c r="BL10" s="14"/>
-      <c r="BM10" s="14"/>
-      <c r="BN10" s="14"/>
-      <c r="BO10" s="13"/>
-      <c r="BP10" s="13"/>
+      <c r="A10" s="51"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="52"/>
+      <c r="J10" s="57"/>
+      <c r="K10" s="58"/>
+      <c r="L10" s="58"/>
+      <c r="M10" s="58"/>
+      <c r="N10" s="59"/>
+      <c r="O10" s="52"/>
+      <c r="P10" s="52"/>
+      <c r="Q10" s="52"/>
+      <c r="R10" s="52"/>
+      <c r="S10" s="52"/>
+      <c r="T10" s="52"/>
+      <c r="U10" s="52"/>
+      <c r="V10" s="52"/>
+      <c r="W10" s="52"/>
+      <c r="X10" s="52"/>
+      <c r="Y10" s="52"/>
+      <c r="Z10" s="52"/>
+      <c r="AA10" s="52"/>
+      <c r="AB10" s="52"/>
+      <c r="AC10" s="52"/>
+      <c r="AD10" s="52"/>
+      <c r="AE10" s="52"/>
+      <c r="AF10" s="52"/>
+      <c r="AG10" s="52"/>
+      <c r="AH10" s="52"/>
+      <c r="AI10" s="52"/>
+      <c r="AJ10" s="52"/>
+      <c r="AK10" s="52"/>
+      <c r="AL10" s="52"/>
+      <c r="AM10" s="52"/>
+      <c r="AN10" s="52"/>
+      <c r="AO10" s="52"/>
+      <c r="AP10" s="52"/>
+      <c r="AQ10" s="52"/>
+      <c r="AR10" s="52"/>
+      <c r="AS10" s="52"/>
+      <c r="AT10" s="52"/>
+      <c r="AU10" s="52"/>
+      <c r="AV10" s="52"/>
+      <c r="AW10" s="52"/>
+      <c r="AX10" s="52"/>
+      <c r="AY10" s="52"/>
+      <c r="AZ10" s="52"/>
+      <c r="BA10" s="52"/>
+      <c r="BB10" s="52"/>
+      <c r="BC10" s="52"/>
+      <c r="BD10" s="54"/>
+      <c r="BE10" s="54"/>
+      <c r="BF10" s="54"/>
+      <c r="BG10" s="55"/>
+      <c r="BH10" s="55"/>
+      <c r="BI10" s="55"/>
+      <c r="BJ10" s="56"/>
+      <c r="BK10" s="56"/>
+      <c r="BL10" s="56"/>
+      <c r="BM10" s="56"/>
+      <c r="BN10" s="56"/>
+      <c r="BO10" s="55"/>
+      <c r="BP10" s="55"/>
     </row>
     <row r="11" spans="1:71" ht="16.2" customHeight="1">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
-      <c r="M11" s="19"/>
-      <c r="N11" s="20"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="15"/>
-      <c r="S11" s="15"/>
-      <c r="T11" s="15"/>
-      <c r="U11" s="15"/>
-      <c r="V11" s="15"/>
-      <c r="W11" s="15"/>
-      <c r="X11" s="15"/>
-      <c r="Y11" s="15"/>
-      <c r="Z11" s="15"/>
-      <c r="AA11" s="15"/>
-      <c r="AB11" s="15"/>
-      <c r="AC11" s="15"/>
-      <c r="AD11" s="15"/>
-      <c r="AE11" s="15"/>
-      <c r="AF11" s="15"/>
-      <c r="AG11" s="15"/>
-      <c r="AH11" s="15"/>
-      <c r="AI11" s="15"/>
-      <c r="AJ11" s="15"/>
-      <c r="AK11" s="15"/>
-      <c r="AL11" s="15"/>
-      <c r="AM11" s="15"/>
-      <c r="AN11" s="15"/>
-      <c r="AO11" s="15"/>
-      <c r="AP11" s="15"/>
-      <c r="AQ11" s="15"/>
-      <c r="AR11" s="15"/>
-      <c r="AS11" s="15"/>
-      <c r="AT11" s="15"/>
-      <c r="AU11" s="15"/>
-      <c r="AV11" s="15"/>
-      <c r="AW11" s="15"/>
-      <c r="AX11" s="15"/>
-      <c r="AY11" s="15"/>
-      <c r="AZ11" s="15"/>
-      <c r="BA11" s="15"/>
-      <c r="BB11" s="15"/>
-      <c r="BC11" s="15"/>
-      <c r="BD11" s="16"/>
-      <c r="BE11" s="16"/>
-      <c r="BF11" s="16"/>
-      <c r="BG11" s="13"/>
-      <c r="BH11" s="13"/>
-      <c r="BI11" s="13"/>
-      <c r="BJ11" s="14"/>
-      <c r="BK11" s="14"/>
-      <c r="BL11" s="14"/>
-      <c r="BM11" s="14"/>
-      <c r="BN11" s="14"/>
-      <c r="BO11" s="13"/>
-      <c r="BP11" s="13"/>
+      <c r="A11" s="51"/>
+      <c r="B11" s="51"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="52"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="58"/>
+      <c r="L11" s="58"/>
+      <c r="M11" s="58"/>
+      <c r="N11" s="59"/>
+      <c r="O11" s="52"/>
+      <c r="P11" s="52"/>
+      <c r="Q11" s="52"/>
+      <c r="R11" s="52"/>
+      <c r="S11" s="52"/>
+      <c r="T11" s="52"/>
+      <c r="U11" s="52"/>
+      <c r="V11" s="52"/>
+      <c r="W11" s="52"/>
+      <c r="X11" s="52"/>
+      <c r="Y11" s="52"/>
+      <c r="Z11" s="52"/>
+      <c r="AA11" s="52"/>
+      <c r="AB11" s="52"/>
+      <c r="AC11" s="52"/>
+      <c r="AD11" s="52"/>
+      <c r="AE11" s="52"/>
+      <c r="AF11" s="52"/>
+      <c r="AG11" s="52"/>
+      <c r="AH11" s="52"/>
+      <c r="AI11" s="52"/>
+      <c r="AJ11" s="52"/>
+      <c r="AK11" s="52"/>
+      <c r="AL11" s="52"/>
+      <c r="AM11" s="52"/>
+      <c r="AN11" s="52"/>
+      <c r="AO11" s="52"/>
+      <c r="AP11" s="52"/>
+      <c r="AQ11" s="52"/>
+      <c r="AR11" s="52"/>
+      <c r="AS11" s="52"/>
+      <c r="AT11" s="52"/>
+      <c r="AU11" s="52"/>
+      <c r="AV11" s="52"/>
+      <c r="AW11" s="52"/>
+      <c r="AX11" s="52"/>
+      <c r="AY11" s="52"/>
+      <c r="AZ11" s="52"/>
+      <c r="BA11" s="52"/>
+      <c r="BB11" s="52"/>
+      <c r="BC11" s="52"/>
+      <c r="BD11" s="54"/>
+      <c r="BE11" s="54"/>
+      <c r="BF11" s="54"/>
+      <c r="BG11" s="55"/>
+      <c r="BH11" s="55"/>
+      <c r="BI11" s="55"/>
+      <c r="BJ11" s="56"/>
+      <c r="BK11" s="56"/>
+      <c r="BL11" s="56"/>
+      <c r="BM11" s="56"/>
+      <c r="BN11" s="56"/>
+      <c r="BO11" s="55"/>
+      <c r="BP11" s="55"/>
     </row>
     <row r="12" spans="1:71" ht="16.2" customHeight="1">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
-      <c r="M12" s="19"/>
-      <c r="N12" s="20"/>
-      <c r="O12" s="15"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="15"/>
-      <c r="S12" s="15"/>
-      <c r="T12" s="15"/>
-      <c r="U12" s="15"/>
-      <c r="V12" s="15"/>
-      <c r="W12" s="15"/>
-      <c r="X12" s="15"/>
-      <c r="Y12" s="15"/>
-      <c r="Z12" s="15"/>
-      <c r="AA12" s="15"/>
-      <c r="AB12" s="15"/>
-      <c r="AC12" s="15"/>
-      <c r="AD12" s="15"/>
-      <c r="AE12" s="15"/>
-      <c r="AF12" s="15"/>
-      <c r="AG12" s="15"/>
-      <c r="AH12" s="15"/>
-      <c r="AI12" s="15"/>
-      <c r="AJ12" s="15"/>
-      <c r="AK12" s="15"/>
-      <c r="AL12" s="15"/>
-      <c r="AM12" s="15"/>
-      <c r="AN12" s="15"/>
-      <c r="AO12" s="15"/>
-      <c r="AP12" s="15"/>
-      <c r="AQ12" s="15"/>
-      <c r="AR12" s="15"/>
-      <c r="AS12" s="15"/>
-      <c r="AT12" s="15"/>
-      <c r="AU12" s="15"/>
-      <c r="AV12" s="15"/>
-      <c r="AW12" s="15"/>
-      <c r="AX12" s="15"/>
-      <c r="AY12" s="15"/>
-      <c r="AZ12" s="15"/>
-      <c r="BA12" s="15"/>
-      <c r="BB12" s="15"/>
-      <c r="BC12" s="15"/>
-      <c r="BD12" s="16"/>
-      <c r="BE12" s="16"/>
-      <c r="BF12" s="16"/>
-      <c r="BG12" s="13"/>
-      <c r="BH12" s="13"/>
-      <c r="BI12" s="13"/>
-      <c r="BJ12" s="14"/>
-      <c r="BK12" s="14"/>
-      <c r="BL12" s="14"/>
-      <c r="BM12" s="14"/>
-      <c r="BN12" s="14"/>
-      <c r="BO12" s="13"/>
-      <c r="BP12" s="13"/>
+      <c r="A12" s="51"/>
+      <c r="B12" s="51"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="52"/>
+      <c r="G12" s="52"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="57"/>
+      <c r="K12" s="58"/>
+      <c r="L12" s="58"/>
+      <c r="M12" s="58"/>
+      <c r="N12" s="59"/>
+      <c r="O12" s="52"/>
+      <c r="P12" s="52"/>
+      <c r="Q12" s="52"/>
+      <c r="R12" s="52"/>
+      <c r="S12" s="52"/>
+      <c r="T12" s="52"/>
+      <c r="U12" s="52"/>
+      <c r="V12" s="52"/>
+      <c r="W12" s="52"/>
+      <c r="X12" s="52"/>
+      <c r="Y12" s="52"/>
+      <c r="Z12" s="52"/>
+      <c r="AA12" s="52"/>
+      <c r="AB12" s="52"/>
+      <c r="AC12" s="52"/>
+      <c r="AD12" s="52"/>
+      <c r="AE12" s="52"/>
+      <c r="AF12" s="52"/>
+      <c r="AG12" s="52"/>
+      <c r="AH12" s="52"/>
+      <c r="AI12" s="52"/>
+      <c r="AJ12" s="52"/>
+      <c r="AK12" s="52"/>
+      <c r="AL12" s="52"/>
+      <c r="AM12" s="52"/>
+      <c r="AN12" s="52"/>
+      <c r="AO12" s="52"/>
+      <c r="AP12" s="52"/>
+      <c r="AQ12" s="52"/>
+      <c r="AR12" s="52"/>
+      <c r="AS12" s="52"/>
+      <c r="AT12" s="52"/>
+      <c r="AU12" s="52"/>
+      <c r="AV12" s="52"/>
+      <c r="AW12" s="52"/>
+      <c r="AX12" s="52"/>
+      <c r="AY12" s="52"/>
+      <c r="AZ12" s="52"/>
+      <c r="BA12" s="52"/>
+      <c r="BB12" s="52"/>
+      <c r="BC12" s="52"/>
+      <c r="BD12" s="54"/>
+      <c r="BE12" s="54"/>
+      <c r="BF12" s="54"/>
+      <c r="BG12" s="55"/>
+      <c r="BH12" s="55"/>
+      <c r="BI12" s="55"/>
+      <c r="BJ12" s="56"/>
+      <c r="BK12" s="56"/>
+      <c r="BL12" s="56"/>
+      <c r="BM12" s="56"/>
+      <c r="BN12" s="56"/>
+      <c r="BO12" s="55"/>
+      <c r="BP12" s="55"/>
     </row>
     <row r="13" spans="1:71" ht="16.2" customHeight="1">
-      <c r="A13" s="17"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="19"/>
-      <c r="M13" s="19"/>
-      <c r="N13" s="20"/>
-      <c r="O13" s="15"/>
-      <c r="P13" s="15"/>
-      <c r="Q13" s="15"/>
-      <c r="R13" s="15"/>
-      <c r="S13" s="15"/>
-      <c r="T13" s="15"/>
-      <c r="U13" s="15"/>
-      <c r="V13" s="15"/>
-      <c r="W13" s="15"/>
-      <c r="X13" s="15"/>
-      <c r="Y13" s="15"/>
-      <c r="Z13" s="15"/>
-      <c r="AA13" s="15"/>
-      <c r="AB13" s="15"/>
-      <c r="AC13" s="15"/>
-      <c r="AD13" s="15"/>
-      <c r="AE13" s="15"/>
-      <c r="AF13" s="15"/>
-      <c r="AG13" s="15"/>
-      <c r="AH13" s="15"/>
-      <c r="AI13" s="15"/>
-      <c r="AJ13" s="15"/>
-      <c r="AK13" s="15"/>
-      <c r="AL13" s="15"/>
-      <c r="AM13" s="15"/>
-      <c r="AN13" s="15"/>
-      <c r="AO13" s="15"/>
-      <c r="AP13" s="15"/>
-      <c r="AQ13" s="15"/>
-      <c r="AR13" s="15"/>
-      <c r="AS13" s="15"/>
-      <c r="AT13" s="15"/>
-      <c r="AU13" s="15"/>
-      <c r="AV13" s="15"/>
-      <c r="AW13" s="15"/>
-      <c r="AX13" s="15"/>
-      <c r="AY13" s="15"/>
-      <c r="AZ13" s="15"/>
-      <c r="BA13" s="15"/>
-      <c r="BB13" s="15"/>
-      <c r="BC13" s="15"/>
-      <c r="BD13" s="16"/>
-      <c r="BE13" s="16"/>
-      <c r="BF13" s="16"/>
-      <c r="BG13" s="13"/>
-      <c r="BH13" s="13"/>
-      <c r="BI13" s="13"/>
-      <c r="BJ13" s="14"/>
-      <c r="BK13" s="14"/>
-      <c r="BL13" s="14"/>
-      <c r="BM13" s="14"/>
-      <c r="BN13" s="14"/>
-      <c r="BO13" s="13"/>
-      <c r="BP13" s="13"/>
+      <c r="A13" s="51"/>
+      <c r="B13" s="51"/>
+      <c r="C13" s="51"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="57"/>
+      <c r="K13" s="58"/>
+      <c r="L13" s="58"/>
+      <c r="M13" s="58"/>
+      <c r="N13" s="59"/>
+      <c r="O13" s="52"/>
+      <c r="P13" s="52"/>
+      <c r="Q13" s="52"/>
+      <c r="R13" s="52"/>
+      <c r="S13" s="52"/>
+      <c r="T13" s="52"/>
+      <c r="U13" s="52"/>
+      <c r="V13" s="52"/>
+      <c r="W13" s="52"/>
+      <c r="X13" s="52"/>
+      <c r="Y13" s="52"/>
+      <c r="Z13" s="52"/>
+      <c r="AA13" s="52"/>
+      <c r="AB13" s="52"/>
+      <c r="AC13" s="52"/>
+      <c r="AD13" s="52"/>
+      <c r="AE13" s="52"/>
+      <c r="AF13" s="52"/>
+      <c r="AG13" s="52"/>
+      <c r="AH13" s="52"/>
+      <c r="AI13" s="52"/>
+      <c r="AJ13" s="52"/>
+      <c r="AK13" s="52"/>
+      <c r="AL13" s="52"/>
+      <c r="AM13" s="52"/>
+      <c r="AN13" s="52"/>
+      <c r="AO13" s="52"/>
+      <c r="AP13" s="52"/>
+      <c r="AQ13" s="52"/>
+      <c r="AR13" s="52"/>
+      <c r="AS13" s="52"/>
+      <c r="AT13" s="52"/>
+      <c r="AU13" s="52"/>
+      <c r="AV13" s="52"/>
+      <c r="AW13" s="52"/>
+      <c r="AX13" s="52"/>
+      <c r="AY13" s="52"/>
+      <c r="AZ13" s="52"/>
+      <c r="BA13" s="52"/>
+      <c r="BB13" s="52"/>
+      <c r="BC13" s="52"/>
+      <c r="BD13" s="54"/>
+      <c r="BE13" s="54"/>
+      <c r="BF13" s="54"/>
+      <c r="BG13" s="55"/>
+      <c r="BH13" s="55"/>
+      <c r="BI13" s="55"/>
+      <c r="BJ13" s="56"/>
+      <c r="BK13" s="56"/>
+      <c r="BL13" s="56"/>
+      <c r="BM13" s="56"/>
+      <c r="BN13" s="56"/>
+      <c r="BO13" s="55"/>
+      <c r="BP13" s="55"/>
     </row>
     <row r="14" spans="1:71" ht="16.2" customHeight="1">
       <c r="A14" s="4"/>
@@ -3998,32 +4124,72 @@
     </row>
   </sheetData>
   <mergeCells count="116">
-    <mergeCell ref="BM1:BP2"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="E4:I4"/>
-    <mergeCell ref="J4:S4"/>
-    <mergeCell ref="T4:AH4"/>
-    <mergeCell ref="AI4:BC4"/>
-    <mergeCell ref="BD4:BF4"/>
-    <mergeCell ref="BG4:BI4"/>
-    <mergeCell ref="BJ4:BK4"/>
-    <mergeCell ref="BL4:BN4"/>
-    <mergeCell ref="A1:Q2"/>
-    <mergeCell ref="R1:W2"/>
-    <mergeCell ref="X1:AZ2"/>
-    <mergeCell ref="BA1:BC2"/>
-    <mergeCell ref="BD1:BI2"/>
-    <mergeCell ref="BJ1:BL2"/>
-    <mergeCell ref="BO4:BP4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="E5:I5"/>
-    <mergeCell ref="J5:N5"/>
-    <mergeCell ref="O5:S5"/>
-    <mergeCell ref="T5:AH5"/>
-    <mergeCell ref="AI5:BC5"/>
-    <mergeCell ref="BD5:BF5"/>
-    <mergeCell ref="BG5:BI5"/>
-    <mergeCell ref="BJ5:BK5"/>
+    <mergeCell ref="BG6:BI6"/>
+    <mergeCell ref="BJ6:BK6"/>
+    <mergeCell ref="BJ7:BK7"/>
+    <mergeCell ref="BL7:BN7"/>
+    <mergeCell ref="BO7:BP7"/>
+    <mergeCell ref="BG8:BI8"/>
+    <mergeCell ref="BJ8:BK8"/>
+    <mergeCell ref="AI8:BC8"/>
+    <mergeCell ref="BD8:BF8"/>
+    <mergeCell ref="BL8:BN8"/>
+    <mergeCell ref="BO8:BP8"/>
+    <mergeCell ref="BD13:BF13"/>
+    <mergeCell ref="BG13:BI13"/>
+    <mergeCell ref="BJ13:BK13"/>
+    <mergeCell ref="BL13:BN13"/>
+    <mergeCell ref="BO13:BP13"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="E13:I13"/>
+    <mergeCell ref="J13:N13"/>
+    <mergeCell ref="O13:S13"/>
+    <mergeCell ref="T13:AH13"/>
+    <mergeCell ref="AI13:BC13"/>
+    <mergeCell ref="AI12:BC12"/>
+    <mergeCell ref="BD12:BF12"/>
+    <mergeCell ref="BG12:BI12"/>
+    <mergeCell ref="BJ12:BK12"/>
+    <mergeCell ref="BL12:BN12"/>
+    <mergeCell ref="BO12:BP12"/>
+    <mergeCell ref="BD11:BF11"/>
+    <mergeCell ref="BG11:BI11"/>
+    <mergeCell ref="BJ11:BK11"/>
+    <mergeCell ref="BL11:BN11"/>
+    <mergeCell ref="BO11:BP11"/>
+    <mergeCell ref="AI11:BC11"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="E12:I12"/>
+    <mergeCell ref="J12:N12"/>
+    <mergeCell ref="O12:S12"/>
+    <mergeCell ref="T12:AH12"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="E11:I11"/>
+    <mergeCell ref="J11:N11"/>
+    <mergeCell ref="O11:S11"/>
+    <mergeCell ref="T11:AH11"/>
+    <mergeCell ref="AI10:BC10"/>
+    <mergeCell ref="BD10:BF10"/>
+    <mergeCell ref="BG10:BI10"/>
+    <mergeCell ref="BJ10:BK10"/>
+    <mergeCell ref="BL10:BN10"/>
+    <mergeCell ref="BO10:BP10"/>
+    <mergeCell ref="BD9:BF9"/>
+    <mergeCell ref="BG9:BI9"/>
+    <mergeCell ref="BJ9:BK9"/>
+    <mergeCell ref="BL9:BN9"/>
+    <mergeCell ref="BO9:BP9"/>
+    <mergeCell ref="AI9:BC9"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="E10:I10"/>
+    <mergeCell ref="J10:N10"/>
+    <mergeCell ref="O10:S10"/>
+    <mergeCell ref="T10:AH10"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="E9:I9"/>
+    <mergeCell ref="J9:N9"/>
+    <mergeCell ref="O9:S9"/>
+    <mergeCell ref="T9:AH9"/>
     <mergeCell ref="BL5:BN5"/>
     <mergeCell ref="BO5:BP5"/>
     <mergeCell ref="A8:D8"/>
@@ -4048,72 +4214,32 @@
     <mergeCell ref="T6:AH6"/>
     <mergeCell ref="AI6:BC6"/>
     <mergeCell ref="BD6:BF6"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="E10:I10"/>
-    <mergeCell ref="J10:N10"/>
-    <mergeCell ref="O10:S10"/>
-    <mergeCell ref="T10:AH10"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="E9:I9"/>
-    <mergeCell ref="J9:N9"/>
-    <mergeCell ref="O9:S9"/>
-    <mergeCell ref="T9:AH9"/>
-    <mergeCell ref="AI10:BC10"/>
-    <mergeCell ref="BD10:BF10"/>
-    <mergeCell ref="BG10:BI10"/>
-    <mergeCell ref="BJ10:BK10"/>
-    <mergeCell ref="BL10:BN10"/>
-    <mergeCell ref="BO10:BP10"/>
-    <mergeCell ref="BD9:BF9"/>
-    <mergeCell ref="BG9:BI9"/>
-    <mergeCell ref="BJ9:BK9"/>
-    <mergeCell ref="BL9:BN9"/>
-    <mergeCell ref="BO9:BP9"/>
-    <mergeCell ref="AI9:BC9"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="E12:I12"/>
-    <mergeCell ref="J12:N12"/>
-    <mergeCell ref="O12:S12"/>
-    <mergeCell ref="T12:AH12"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="E11:I11"/>
-    <mergeCell ref="J11:N11"/>
-    <mergeCell ref="O11:S11"/>
-    <mergeCell ref="T11:AH11"/>
-    <mergeCell ref="AI12:BC12"/>
-    <mergeCell ref="BD12:BF12"/>
-    <mergeCell ref="BG12:BI12"/>
-    <mergeCell ref="BJ12:BK12"/>
-    <mergeCell ref="BL12:BN12"/>
-    <mergeCell ref="BO12:BP12"/>
-    <mergeCell ref="BD11:BF11"/>
-    <mergeCell ref="BG11:BI11"/>
-    <mergeCell ref="BJ11:BK11"/>
-    <mergeCell ref="BL11:BN11"/>
-    <mergeCell ref="BO11:BP11"/>
-    <mergeCell ref="AI11:BC11"/>
-    <mergeCell ref="BD13:BF13"/>
-    <mergeCell ref="BG13:BI13"/>
-    <mergeCell ref="BJ13:BK13"/>
-    <mergeCell ref="BL13:BN13"/>
-    <mergeCell ref="BO13:BP13"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="E13:I13"/>
-    <mergeCell ref="J13:N13"/>
-    <mergeCell ref="O13:S13"/>
-    <mergeCell ref="T13:AH13"/>
-    <mergeCell ref="AI13:BC13"/>
-    <mergeCell ref="BG6:BI6"/>
-    <mergeCell ref="BJ6:BK6"/>
-    <mergeCell ref="BJ7:BK7"/>
-    <mergeCell ref="BL7:BN7"/>
-    <mergeCell ref="BO7:BP7"/>
-    <mergeCell ref="BG8:BI8"/>
-    <mergeCell ref="BJ8:BK8"/>
-    <mergeCell ref="AI8:BC8"/>
-    <mergeCell ref="BD8:BF8"/>
-    <mergeCell ref="BL8:BN8"/>
-    <mergeCell ref="BO8:BP8"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="E5:I5"/>
+    <mergeCell ref="J5:N5"/>
+    <mergeCell ref="O5:S5"/>
+    <mergeCell ref="T5:AH5"/>
+    <mergeCell ref="AI5:BC5"/>
+    <mergeCell ref="BD5:BF5"/>
+    <mergeCell ref="BG5:BI5"/>
+    <mergeCell ref="BJ5:BK5"/>
+    <mergeCell ref="BM1:BP2"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="J4:S4"/>
+    <mergeCell ref="T4:AH4"/>
+    <mergeCell ref="AI4:BC4"/>
+    <mergeCell ref="BD4:BF4"/>
+    <mergeCell ref="BG4:BI4"/>
+    <mergeCell ref="BJ4:BK4"/>
+    <mergeCell ref="BL4:BN4"/>
+    <mergeCell ref="A1:Q2"/>
+    <mergeCell ref="R1:W2"/>
+    <mergeCell ref="X1:AZ2"/>
+    <mergeCell ref="BA1:BC2"/>
+    <mergeCell ref="BD1:BI2"/>
+    <mergeCell ref="BJ1:BL2"/>
+    <mergeCell ref="BO4:BP4"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4127,11 +4253,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="C4:DS5"/>
+  <dimension ref="C4:DS60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BC4" sqref="BC4:BL5"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N59" sqref="N59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="16.2" customHeight="1"/>
@@ -4304,6 +4430,25 @@
       <c r="DR5" s="61"/>
       <c r="DS5" s="61"/>
     </row>
+    <row r="33" spans="4:56" ht="22.2" customHeight="1">
+      <c r="D33" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="O33" s="65" t="s">
+        <v>42</v>
+      </c>
+      <c r="BA33" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="BD33" s="66" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="60" spans="4:4" ht="16.2" customHeight="1">
+      <c r="D60" s="65" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="CO4:DA5"/>

</xml_diff>